<commit_message>
Merged PR 3624: Merge feature/PRI6134 to develop
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ProprietaryDataFiles/Syndication_ValidFile1.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ProprietaryDataFiles/Syndication_ValidFile1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oleksandr\Desktop\data files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bbotelho\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\ProprietaryDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6B2A90E1-4671-4F19-AE09-F1285F349D57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Barter Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -96,18 +97,6 @@
     <t>Avg HH CPM</t>
   </si>
   <si>
-    <t>P 25-54 Avg Rtg</t>
-  </si>
-  <si>
-    <t>P 25-54 Avg Imps (000)</t>
-  </si>
-  <si>
-    <t>P 25-54 VPVH</t>
-  </si>
-  <si>
-    <t>P 25-54 CPM</t>
-  </si>
-  <si>
     <t>American Dad</t>
   </si>
   <si>
@@ -167,11 +156,23 @@
   <si>
     <t>Cleveland/King of the Hill Combo</t>
   </si>
+  <si>
+    <t>A 18-34 Avg Imps (000)</t>
+  </si>
+  <si>
+    <t>A 18-34 VPVH</t>
+  </si>
+  <si>
+    <t>A 18-34 CPM</t>
+  </si>
+  <si>
+    <t>A 18-34 Avg Rtg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -658,7 +659,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
     <dxf>
@@ -1269,12 +1270,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+      <pane ySplit="15" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
@@ -1777,16 +1778,16 @@
         <v>24</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="J15" s="23"/>
       <c r="K15" s="23"/>
@@ -1800,9 +1801,11 @@
     </row>
     <row r="16" spans="1:26" ht="24" customHeight="1">
       <c r="A16" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="17">
+        <v>10</v>
+      </c>
       <c r="C16" s="17">
         <v>0.62</v>
       </c>
@@ -1844,9 +1847,11 @@
     </row>
     <row r="17" spans="1:26" ht="24" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>20</v>
+      </c>
       <c r="C17" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -1888,9 +1893,11 @@
     </row>
     <row r="18" spans="1:26" ht="24" customHeight="1">
       <c r="A18" s="17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="17">
+        <v>30</v>
+      </c>
       <c r="C18" s="17">
         <v>1.58</v>
       </c>
@@ -1932,9 +1939,11 @@
     </row>
     <row r="19" spans="1:26" ht="24" customHeight="1">
       <c r="A19" s="17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
-      <c r="B19" s="17"/>
+      <c r="B19" s="17">
+        <v>2</v>
+      </c>
       <c r="C19" s="17">
         <v>0.56999999999999995</v>
       </c>
@@ -1976,9 +1985,11 @@
     </row>
     <row r="20" spans="1:26" ht="24" customHeight="1">
       <c r="A20" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
-      <c r="B20" s="17"/>
+      <c r="B20" s="17">
+        <v>5</v>
+      </c>
       <c r="C20" s="17">
         <v>1</v>
       </c>
@@ -2020,9 +2031,11 @@
     </row>
     <row r="21" spans="1:26" ht="24" customHeight="1">
       <c r="A21" s="17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
-      <c r="B21" s="17"/>
+      <c r="B21" s="17">
+        <v>6</v>
+      </c>
       <c r="C21" s="17">
         <v>0.78</v>
       </c>
@@ -2064,9 +2077,11 @@
     </row>
     <row r="22" spans="1:26" ht="24" customHeight="1">
       <c r="A22" s="17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
-      <c r="B22" s="17"/>
+      <c r="B22" s="17">
+        <v>7</v>
+      </c>
       <c r="C22" s="17">
         <v>0.78</v>
       </c>
@@ -2108,9 +2123,11 @@
     </row>
     <row r="23" spans="1:26" ht="24" customHeight="1">
       <c r="A23" s="17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
-      <c r="B23" s="17"/>
+      <c r="B23" s="17">
+        <v>8</v>
+      </c>
       <c r="C23" s="17">
         <v>6.31</v>
       </c>
@@ -2152,9 +2169,11 @@
     </row>
     <row r="24" spans="1:26" ht="24" customHeight="1">
       <c r="A24" s="17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
-      <c r="B24" s="17"/>
+      <c r="B24" s="17">
+        <v>55</v>
+      </c>
       <c r="C24" s="17">
         <v>3.34</v>
       </c>
@@ -2196,9 +2215,11 @@
     </row>
     <row r="25" spans="1:26" ht="24" customHeight="1">
       <c r="A25" s="17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
-      <c r="B25" s="17"/>
+      <c r="B25" s="17">
+        <v>99</v>
+      </c>
       <c r="C25" s="17">
         <v>1.44</v>
       </c>
@@ -2240,9 +2261,11 @@
     </row>
     <row r="26" spans="1:26" ht="24" customHeight="1">
       <c r="A26" s="17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="17">
+        <v>1</v>
+      </c>
       <c r="C26" s="17">
         <v>1.42</v>
       </c>
@@ -2284,9 +2307,11 @@
     </row>
     <row r="27" spans="1:26" ht="24" customHeight="1">
       <c r="A27" s="17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
-      <c r="B27" s="17"/>
+      <c r="B27" s="17">
+        <v>1</v>
+      </c>
       <c r="C27" s="17">
         <v>0.76</v>
       </c>
@@ -2328,9 +2353,11 @@
     </row>
     <row r="28" spans="1:26" ht="24" customHeight="1">
       <c r="A28" s="17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="17">
+        <v>10</v>
+      </c>
       <c r="C28" s="17">
         <v>2.0299999999999998</v>
       </c>
@@ -2372,9 +2399,11 @@
     </row>
     <row r="29" spans="1:26" ht="24" customHeight="1">
       <c r="A29" s="17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
-      <c r="B29" s="17"/>
+      <c r="B29" s="17">
+        <v>5</v>
+      </c>
       <c r="C29" s="17">
         <v>1.39</v>
       </c>
@@ -2416,9 +2445,11 @@
     </row>
     <row r="30" spans="1:26" ht="24" customHeight="1">
       <c r="A30" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
-      <c r="B30" s="17"/>
+      <c r="B30" s="17">
+        <v>9</v>
+      </c>
       <c r="C30" s="17">
         <v>2.12</v>
       </c>
@@ -2460,9 +2491,11 @@
     </row>
     <row r="31" spans="1:26" ht="24" customHeight="1">
       <c r="A31" s="17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
-      <c r="B31" s="17"/>
+      <c r="B31" s="17">
+        <v>6</v>
+      </c>
       <c r="C31" s="17">
         <v>2.29</v>
       </c>
@@ -2504,9 +2537,11 @@
     </row>
     <row r="32" spans="1:26" ht="24" customHeight="1">
       <c r="A32" s="17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
-      <c r="B32" s="17"/>
+      <c r="B32" s="17">
+        <v>8</v>
+      </c>
       <c r="C32" s="17">
         <v>0.71</v>
       </c>
@@ -2548,9 +2583,11 @@
     </row>
     <row r="33" spans="1:26" ht="24" customHeight="1">
       <c r="A33" s="17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
-      <c r="B33" s="17"/>
+      <c r="B33" s="17">
+        <v>8</v>
+      </c>
       <c r="C33" s="17">
         <v>1</v>
       </c>
@@ -2592,9 +2629,11 @@
     </row>
     <row r="34" spans="1:26" ht="24" customHeight="1">
       <c r="A34" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
-      <c r="B34" s="17"/>
+      <c r="B34" s="17">
+        <v>6</v>
+      </c>
       <c r="C34" s="17">
         <v>1.1499999999999999</v>
       </c>
@@ -2636,9 +2675,11 @@
     </row>
     <row r="35" spans="1:26" ht="24" customHeight="1">
       <c r="A35" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
-      <c r="B35" s="17"/>
+      <c r="B35" s="17">
+        <v>10</v>
+      </c>
       <c r="C35" s="17">
         <v>0.46</v>
       </c>
@@ -29865,22 +29906,22 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Inventory Source - The inventory source you entered is unknown.  _x000a__x000a_Please select an existing source from the dropdown or contact support to add the inventory source." sqref="B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Inventory Source - The inventory source you entered is unknown.  _x000a__x000a_Please select an existing source from the dropdown or contact support to add the inventory source." sqref="B3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"20th Century Fox (Twentieth Century),CBS Synd,NBCU Syn,WB Syn"</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="B4">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>B4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Daypart Code - The daypart code you entered is unknown.  _x000a__x000a_Please select an existing daypart code from the dropdown or contact support to add the daypart code." sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Daypart Code - The daypart code you entered is unknown.  _x000a__x000a_Please select an existing daypart code from the dropdown or contact support to add the daypart code." sqref="B6" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"SYN"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Playback Type - The playback type you entered is unknown.  _x000a__x000a_Please select an existing playback type from the dropdown or contact support to add the playback type." sqref="B10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Unknown Playback Type - The playback type you entered is unknown.  _x000a__x000a_Please select an existing playback type from the dropdown or contact support to add the playback type." sqref="B10" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Live,Live+S,Live+1,Live+3,Live+7"</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8 B9">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8 B9" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>